<commit_message>
Tested 2 tests, added some tests
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
@@ -5,18 +5,18 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewaston\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Test Plan" sheetId="1" r:id="rId1"/>
     <sheet name="-Disclaimer-" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Test Plan'!$B$2:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Test Plan'!$B$2:$J$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>TESTER COMMENTS</t>
   </si>
@@ -133,6 +133,33 @@
   </si>
   <si>
     <t>Calculate all valid locations based on Cost restriction and show on screen(*x money, 023 search)</t>
+  </si>
+  <si>
+    <t>Two Search boxes show up on screen</t>
+  </si>
+  <si>
+    <t>Afzal</t>
+  </si>
+  <si>
+    <t>Gap between Search and filter buttons no consistent with gap between search boxes</t>
+  </si>
+  <si>
+    <t>Run SSIS package to load file contents into database</t>
+  </si>
+  <si>
+    <t>Database to have same number of entries in it as CSV file</t>
+  </si>
+  <si>
+    <t>Search with both search bars(023, first search bar), (heart, second search bar), one after the other.</t>
+  </si>
+  <si>
+    <t>Correct data on screen for earch search bar search.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct data shows as expected on screen with both search bars working. </t>
+  </si>
+  <si>
+    <t>When using both search bars simoultanously, it returns null with no entries right now(possible new task)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +462,55 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <strike/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -854,7 +929,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -903,6 +978,10 @@
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$25" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1071,13 +1150,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1138,13 +1217,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1205,13 +1284,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1272,13 +1351,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>12</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1339,13 +1418,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1406,13 +1485,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1473,13 +1552,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>14</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>14</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1540,13 +1619,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1607,13 +1686,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1674,13 +1753,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1741,13 +1820,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1808,13 +1887,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1875,13 +1954,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1936,64 +2015,19 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>706</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>78820</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15913100" y="0"/>
-          <a:ext cx="3321756" cy="650320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2054,13 +2088,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2121,13 +2155,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2188,13 +2222,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>24</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2255,13 +2289,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>25</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2322,13 +2356,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>26</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>26</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2389,13 +2423,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>27</xdr:row>
+          <xdr:row>28</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>27</xdr:row>
+          <xdr:row>28</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2456,13 +2490,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>28</xdr:row>
+          <xdr:row>29</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>28</xdr:row>
+          <xdr:row>29</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2523,13 +2557,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>30</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2590,13 +2624,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>31</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2657,13 +2691,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2724,13 +2758,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>33</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>33</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2791,13 +2825,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>33</xdr:row>
+          <xdr:row>34</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>33</xdr:row>
+          <xdr:row>34</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2858,13 +2892,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>34</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>34</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2925,13 +2959,13 @@
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
-          <xdr:row>35</xdr:row>
+          <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>35</xdr:row>
+          <xdr:row>36</xdr:row>
           <xdr:rowOff>285750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2983,6 +3017,68 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>647700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="400050" cy="247650"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1144" name="Check Box 120" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1144"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3315,11 +3411,11 @@
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Y74"/>
+  <dimension ref="B1:Y75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3574,10 +3670,16 @@
       <c r="F8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -3599,21 +3701,27 @@
         <v>43865</v>
       </c>
       <c r="C9" s="25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="15"/>
+        <v>41</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="H9" s="16"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="I9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -3635,16 +3743,16 @@
         <v>43865</v>
       </c>
       <c r="C10" s="25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10" s="15">
         <v>1</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="16"/>
@@ -3671,16 +3779,16 @@
         <v>43865</v>
       </c>
       <c r="C11" s="25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="15">
         <v>1</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="16"/>
@@ -3707,16 +3815,16 @@
         <v>43865</v>
       </c>
       <c r="C12" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="15">
         <v>1</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
@@ -3746,13 +3854,13 @@
         <v>4</v>
       </c>
       <c r="D13" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="16"/>
@@ -3779,16 +3887,16 @@
         <v>43865</v>
       </c>
       <c r="C14" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="16"/>
@@ -3812,19 +3920,19 @@
     </row>
     <row r="15" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14">
-        <v>43274</v>
+        <v>43865</v>
       </c>
       <c r="C15" s="25">
         <v>3</v>
       </c>
       <c r="D15" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="16"/>
@@ -3848,12 +3956,20 @@
     </row>
     <row r="16" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
-        <v>43275</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+        <v>43274</v>
+      </c>
+      <c r="C16" s="25">
+        <v>3</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="16"/>
       <c r="I16" s="15"/>
@@ -3874,14 +3990,22 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
-        <v>43276</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+        <v>43275</v>
+      </c>
+      <c r="C17" s="25">
+        <v>7</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
       <c r="I17" s="15"/>
@@ -3904,7 +4028,7 @@
     </row>
     <row r="18" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
-        <v>43277</v>
+        <v>43276</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="15"/>
@@ -3932,7 +4056,7 @@
     </row>
     <row r="19" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14">
-        <v>43278</v>
+        <v>43277</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="15"/>
@@ -3960,7 +4084,7 @@
     </row>
     <row r="20" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="14">
-        <v>43279</v>
+        <v>43278</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="15"/>
@@ -3988,7 +4112,7 @@
     </row>
     <row r="21" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="14">
-        <v>43280</v>
+        <v>43279</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="15"/>
@@ -4016,7 +4140,7 @@
     </row>
     <row r="22" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="14">
-        <v>43281</v>
+        <v>43280</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="15"/>
@@ -4044,7 +4168,7 @@
     </row>
     <row r="23" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14">
-        <v>43282</v>
+        <v>43281</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="15"/>
@@ -4072,7 +4196,7 @@
     </row>
     <row r="24" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14">
-        <v>43283</v>
+        <v>43282</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="15"/>
@@ -4100,7 +4224,7 @@
     </row>
     <row r="25" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14">
-        <v>43284</v>
+        <v>43283</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="15"/>
@@ -4128,7 +4252,7 @@
     </row>
     <row r="26" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="14">
-        <v>43285</v>
+        <v>43284</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="15"/>
@@ -4156,7 +4280,7 @@
     </row>
     <row r="27" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14">
-        <v>43286</v>
+        <v>43285</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="15"/>
@@ -4184,7 +4308,7 @@
     </row>
     <row r="28" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14">
-        <v>43287</v>
+        <v>43286</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="15"/>
@@ -4212,7 +4336,7 @@
     </row>
     <row r="29" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14">
-        <v>43288</v>
+        <v>43287</v>
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="15"/>
@@ -4240,7 +4364,7 @@
     </row>
     <row r="30" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14">
-        <v>43289</v>
+        <v>43288</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="15"/>
@@ -4268,7 +4392,7 @@
     </row>
     <row r="31" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14">
-        <v>43290</v>
+        <v>43289</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="15"/>
@@ -4296,7 +4420,7 @@
     </row>
     <row r="32" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14">
-        <v>43291</v>
+        <v>43290</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="15"/>
@@ -4324,7 +4448,7 @@
     </row>
     <row r="33" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14">
-        <v>43292</v>
+        <v>43291</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="15"/>
@@ -4352,7 +4476,7 @@
     </row>
     <row r="34" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
-        <v>43293</v>
+        <v>43292</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="15"/>
@@ -4380,7 +4504,7 @@
     </row>
     <row r="35" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14">
-        <v>43294</v>
+        <v>43293</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="15"/>
@@ -4408,7 +4532,7 @@
     </row>
     <row r="36" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14">
-        <v>43295</v>
+        <v>43294</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="15"/>
@@ -4434,18 +4558,18 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
     </row>
-    <row r="37" spans="2:25" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14">
-        <v>43296</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+        <v>43295</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -4462,59 +4586,61 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
     </row>
-    <row r="38" spans="2:25" s="19" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="32" t="s">
+    <row r="38" spans="2:25" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="14">
+        <v>43296</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" spans="2:25" s="19" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="17"/>
-      <c r="S38" s="17"/>
-      <c r="T38" s="17"/>
-      <c r="U38" s="17"/>
-      <c r="V38" s="17"/>
-      <c r="W38" s="17"/>
-      <c r="X38" s="17"/>
-      <c r="Y38" s="17"/>
-    </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-      <c r="Y39" s="1"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5426,12 +5552,38 @@
       <c r="X74" s="1"/>
       <c r="Y74" s="1"/>
     </row>
+    <row r="75" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B38:J38"/>
+    <mergeCell ref="B39:J39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B38:J38" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET"/>
+    <hyperlink ref="B39:J39" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET"/>
   </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -5492,28 +5644,6 @@
                   <from>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>647700</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1084" r:id="rId8" name="Check Box 60">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>7</xdr:col>
-                    <xdr:colOff>647700</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </from>
@@ -5530,7 +5660,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1085" r:id="rId9" name="Check Box 61">
+            <control shapeId="1084" r:id="rId8" name="Check Box 60">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5552,7 +5682,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1086" r:id="rId10" name="Check Box 62">
+            <control shapeId="1085" r:id="rId9" name="Check Box 61">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5574,7 +5704,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1087" r:id="rId11" name="Check Box 63">
+            <control shapeId="1086" r:id="rId10" name="Check Box 62">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5596,7 +5726,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1088" r:id="rId12" name="Check Box 64">
+            <control shapeId="1087" r:id="rId11" name="Check Box 63">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5618,7 +5748,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1089" r:id="rId13" name="Check Box 65">
+            <control shapeId="1088" r:id="rId12" name="Check Box 64">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5640,7 +5770,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1090" r:id="rId14" name="Check Box 66">
+            <control shapeId="1089" r:id="rId13" name="Check Box 65">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5662,7 +5792,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1091" r:id="rId15" name="Check Box 67">
+            <control shapeId="1090" r:id="rId14" name="Check Box 66">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5684,7 +5814,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1092" r:id="rId16" name="Check Box 68">
+            <control shapeId="1091" r:id="rId15" name="Check Box 67">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5706,7 +5836,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1093" r:id="rId17" name="Check Box 69">
+            <control shapeId="1092" r:id="rId16" name="Check Box 68">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5728,7 +5858,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1094" r:id="rId18" name="Check Box 70">
+            <control shapeId="1093" r:id="rId17" name="Check Box 69">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5750,7 +5880,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1095" r:id="rId19" name="Check Box 71">
+            <control shapeId="1094" r:id="rId18" name="Check Box 70">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5772,7 +5902,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1128" r:id="rId20" name="Check Box 104">
+            <control shapeId="1095" r:id="rId19" name="Check Box 71">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5794,7 +5924,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1129" r:id="rId21" name="Check Box 105">
+            <control shapeId="1128" r:id="rId20" name="Check Box 104">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5816,7 +5946,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1130" r:id="rId22" name="Check Box 106">
+            <control shapeId="1129" r:id="rId21" name="Check Box 105">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5838,7 +5968,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1131" r:id="rId23" name="Check Box 107">
+            <control shapeId="1130" r:id="rId22" name="Check Box 106">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5860,7 +5990,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1132" r:id="rId24" name="Check Box 108">
+            <control shapeId="1131" r:id="rId23" name="Check Box 107">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5882,7 +6012,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1133" r:id="rId25" name="Check Box 109">
+            <control shapeId="1132" r:id="rId24" name="Check Box 108">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5904,7 +6034,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1134" r:id="rId26" name="Check Box 110">
+            <control shapeId="1133" r:id="rId25" name="Check Box 109">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5926,7 +6056,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1135" r:id="rId27" name="Check Box 111">
+            <control shapeId="1134" r:id="rId26" name="Check Box 110">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5948,7 +6078,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1136" r:id="rId28" name="Check Box 112">
+            <control shapeId="1135" r:id="rId27" name="Check Box 111">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5970,7 +6100,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1137" r:id="rId29" name="Check Box 113">
+            <control shapeId="1136" r:id="rId28" name="Check Box 112">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5992,7 +6122,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1138" r:id="rId30" name="Check Box 114">
+            <control shapeId="1137" r:id="rId29" name="Check Box 113">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -6014,7 +6144,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1139" r:id="rId31" name="Check Box 115">
+            <control shapeId="1138" r:id="rId30" name="Check Box 114">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -6036,7 +6166,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1140" r:id="rId32" name="Check Box 116">
+            <control shapeId="1139" r:id="rId31" name="Check Box 115">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -6058,7 +6188,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1141" r:id="rId33" name="Check Box 117">
+            <control shapeId="1140" r:id="rId32" name="Check Box 116">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -6080,7 +6210,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1142" r:id="rId34" name="Check Box 118">
+            <control shapeId="1141" r:id="rId33" name="Check Box 117">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -6100,6 +6230,50 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1142" r:id="rId34" name="Check Box 118">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>647700</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1144" r:id="rId35" name="Check Box 120">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>647700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -6107,7 +6281,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="63" id="{FFFD2BF5-B923-6D47-B6E7-3734A4AC39E2}">
+          <x14:cfRule type="expression" priority="65" id="{FFFD2BF5-B923-6D47-B6E7-3734A4AC39E2}">
             <xm:f>'-Disclaimer-'!$A$12=TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -6122,10 +6296,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C8:H8 C9:C29</xm:sqref>
+          <xm:sqref>C8:H8 C10:C30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="62" id="{07E4F01B-CE26-5B4D-ACF3-1E0A8EB2FD23}">
+          <x14:cfRule type="expression" priority="64" id="{07E4F01B-CE26-5B4D-ACF3-1E0A8EB2FD23}">
             <xm:f>'-Disclaimer-'!$A$11=TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -6140,10 +6314,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B7:J7 I8:J9 B8:B37</xm:sqref>
+          <xm:sqref>B7:J7 I8:J8 B8 B10:B38 I10:J10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="61" id="{1C4D6E8F-045C-5F4C-B1D8-7ABA82174623}">
+          <x14:cfRule type="expression" priority="63" id="{1C4D6E8F-045C-5F4C-B1D8-7ABA82174623}">
             <xm:f>'-Disclaimer-'!$A$13=TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -6158,29 +6332,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D9:H9</xm:sqref>
+          <xm:sqref>D10:H10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{1C67D2DD-76C7-1A4A-AD82-AD7BCE7F3721}">
+          <x14:cfRule type="expression" priority="62" id="{1C67D2DD-76C7-1A4A-AD82-AD7BCE7F3721}">
             <xm:f>'-Disclaimer-'!$A$14=TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <strike/>
-                <color auto="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="none">
-                  <fgColor indexed="64"/>
-                  <bgColor auto="1"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D10:J10</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="59" id="{D9C53A36-BD51-AC46-A4F2-6C62EDDE7121}">
-            <xm:f>'-Disclaimer-'!$A$15=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6197,8 +6353,8 @@
           <xm:sqref>D11:J11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="58" id="{8FC70330-4439-C348-A01B-5213FE7A2476}">
-            <xm:f>'-Disclaimer-'!$A$16=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="61" id="{D9C53A36-BD51-AC46-A4F2-6C62EDDE7121}">
+            <xm:f>'-Disclaimer-'!$A$15=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6215,8 +6371,8 @@
           <xm:sqref>D12:J12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{7DE95375-D593-484E-AE75-B1DEE5A8DB67}">
-            <xm:f>'-Disclaimer-'!$A$17=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="60" id="{8FC70330-4439-C348-A01B-5213FE7A2476}">
+            <xm:f>'-Disclaimer-'!$A$16=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6233,8 +6389,8 @@
           <xm:sqref>D13:J13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="56" id="{AD64F53D-8676-514D-9BD9-E801A993A1F0}">
-            <xm:f>'-Disclaimer-'!$A$18=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="59" id="{7DE95375-D593-484E-AE75-B1DEE5A8DB67}">
+            <xm:f>'-Disclaimer-'!$A$17=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6251,8 +6407,8 @@
           <xm:sqref>D14:J14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="55" id="{5334E948-3CD8-8D4E-8D9E-7FE9FABDCF69}">
-            <xm:f>'-Disclaimer-'!$A$19=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="58" id="{AD64F53D-8676-514D-9BD9-E801A993A1F0}">
+            <xm:f>'-Disclaimer-'!$A$18=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6269,8 +6425,8 @@
           <xm:sqref>D15:J15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="54" id="{A43819E2-9E91-D94D-BB25-339DBBD7AE17}">
-            <xm:f>'-Disclaimer-'!$A$20=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="57" id="{5334E948-3CD8-8D4E-8D9E-7FE9FABDCF69}">
+            <xm:f>'-Disclaimer-'!$A$19=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6287,8 +6443,8 @@
           <xm:sqref>D16:J16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="53" id="{6F3D8FCE-584C-DA4F-94E0-366571699CA0}">
-            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="56" id="{A43819E2-9E91-D94D-BB25-339DBBD7AE17}">
+            <xm:f>'-Disclaimer-'!$A$20=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6305,8 +6461,8 @@
           <xm:sqref>D17:J17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="52" id="{9737A92A-FEF4-CA4F-B314-425F576BBD4E}">
-            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="55" id="{6F3D8FCE-584C-DA4F-94E0-366571699CA0}">
+            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6323,8 +6479,8 @@
           <xm:sqref>D18:J18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="51" id="{F9A293A6-9690-7E4C-A267-218913D00132}">
-            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="54" id="{9737A92A-FEF4-CA4F-B314-425F576BBD4E}">
+            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6341,8 +6497,8 @@
           <xm:sqref>D19:J19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="50" id="{82CAD8AD-3630-274D-9078-503929890D3E}">
-            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="53" id="{F9A293A6-9690-7E4C-A267-218913D00132}">
+            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6359,8 +6515,8 @@
           <xm:sqref>D20:J20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="49" id="{0B1A353E-5A08-3A44-A7CC-7C117EDA363D}">
-            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="52" id="{82CAD8AD-3630-274D-9078-503929890D3E}">
+            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6377,8 +6533,8 @@
           <xm:sqref>D21:J21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="15" id="{1CB154C3-B5D9-6C41-BE32-8DA2EC0756D3}">
-            <xm:f>'-Disclaimer-'!$A$16=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="51" id="{0B1A353E-5A08-3A44-A7CC-7C117EDA363D}">
+            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6395,8 +6551,8 @@
           <xm:sqref>D22:J22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="14" id="{94AF9E3A-33F7-1343-A4B3-D9349C732A05}">
-            <xm:f>'-Disclaimer-'!$A$17=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="17" id="{1CB154C3-B5D9-6C41-BE32-8DA2EC0756D3}">
+            <xm:f>'-Disclaimer-'!$A$16=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6413,8 +6569,8 @@
           <xm:sqref>D23:J23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="13" id="{D2F09604-3EAE-A640-AA5D-4FA96B592FE1}">
-            <xm:f>'-Disclaimer-'!$A$18=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="16" id="{94AF9E3A-33F7-1343-A4B3-D9349C732A05}">
+            <xm:f>'-Disclaimer-'!$A$17=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6431,8 +6587,8 @@
           <xm:sqref>D24:J24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="12" id="{47860E42-1404-4641-A63E-F9F3C18CB933}">
-            <xm:f>'-Disclaimer-'!$A$19=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="15" id="{D2F09604-3EAE-A640-AA5D-4FA96B592FE1}">
+            <xm:f>'-Disclaimer-'!$A$18=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6449,8 +6605,8 @@
           <xm:sqref>D25:J25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{5B69AFB5-67DA-D646-95FE-06CA8930447A}">
-            <xm:f>'-Disclaimer-'!$A$20=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="14" id="{47860E42-1404-4641-A63E-F9F3C18CB933}">
+            <xm:f>'-Disclaimer-'!$A$19=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6467,8 +6623,8 @@
           <xm:sqref>D26:J26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="10" id="{36588A08-5E10-3A4A-8DE2-199A939DF05A}">
-            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="13" id="{5B69AFB5-67DA-D646-95FE-06CA8930447A}">
+            <xm:f>'-Disclaimer-'!$A$20=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6485,8 +6641,8 @@
           <xm:sqref>D27:J27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{EF2DD601-5804-8240-A829-2E220F9F07B9}">
-            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="12" id="{36588A08-5E10-3A4A-8DE2-199A939DF05A}">
+            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6503,8 +6659,8 @@
           <xm:sqref>D28:J28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{A0961B56-CB64-294B-A780-0E9C65C1E1DA}">
-            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="11" id="{EF2DD601-5804-8240-A829-2E220F9F07B9}">
+            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6521,8 +6677,8 @@
           <xm:sqref>D29:J29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{FB0EDD02-3F50-7547-9667-5CEBC77D2AA4}">
-            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="10" id="{A0961B56-CB64-294B-A780-0E9C65C1E1DA}">
+            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6536,11 +6692,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C30:J30</xm:sqref>
+          <xm:sqref>D30:J30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{AA4AF220-320C-344F-B90B-03F5C4D7EDE5}">
-            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="9" id="{FB0EDD02-3F50-7547-9667-5CEBC77D2AA4}">
+            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6557,8 +6713,8 @@
           <xm:sqref>C31:J31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{189503CF-D475-AF46-86B4-540796B8524A}">
-            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="8" id="{AA4AF220-320C-344F-B90B-03F5C4D7EDE5}">
+            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6575,8 +6731,8 @@
           <xm:sqref>C32:J32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{BA8425F0-C9E3-3545-876E-37844D07E0BA}">
-            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="7" id="{189503CF-D475-AF46-86B4-540796B8524A}">
+            <xm:f>'-Disclaimer-'!$A$21=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6593,8 +6749,8 @@
           <xm:sqref>C33:J33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{7CDB6807-DE8A-7646-8280-7BBB132CF999}">
-            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="6" id="{BA8425F0-C9E3-3545-876E-37844D07E0BA}">
+            <xm:f>'-Disclaimer-'!$A$22=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6611,8 +6767,8 @@
           <xm:sqref>C34:J34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{6FC37A1F-EDA1-7F4C-8D02-F70B6BA267F9}">
-            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="5" id="{7CDB6807-DE8A-7646-8280-7BBB132CF999}">
+            <xm:f>'-Disclaimer-'!$A$23=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6629,8 +6785,8 @@
           <xm:sqref>C35:J35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{E654506E-FD4C-FB48-9F34-EE37ADC0E754}">
-            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
+          <x14:cfRule type="expression" priority="4" id="{6FC37A1F-EDA1-7F4C-8D02-F70B6BA267F9}">
+            <xm:f>'-Disclaimer-'!$A$24=TRUE</xm:f>
             <x14:dxf>
               <font>
                 <strike/>
@@ -6646,6 +6802,60 @@
           </x14:cfRule>
           <xm:sqref>C36:J36</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{E654506E-FD4C-FB48-9F34-EE37ADC0E754}">
+            <xm:f>'-Disclaimer-'!$A$25=TRUE</xm:f>
+            <x14:dxf>
+              <font>
+                <strike/>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <fgColor indexed="64"/>
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C37:J37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{CA21BE1F-CE2C-4352-A508-586FDA000F3B}">
+            <xm:f>'-Disclaimer-'!$A$12=TRUE</xm:f>
+            <x14:dxf>
+              <font>
+                <strike/>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <fgColor indexed="64"/>
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C9:H9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{A15E482A-DD82-4D06-BEA6-5FE60B7A22CE}">
+            <xm:f>'-Disclaimer-'!$A$11=TRUE</xm:f>
+            <x14:dxf>
+              <font>
+                <strike/>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <fgColor indexed="64"/>
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I9:J9 B9</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6660,7 +6870,7 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:B14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -6685,11 +6895,16 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6705,12 +6920,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E699AB3B5B90B4E9587B6CE8A7722F9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327bf17b6c8b56faa046bfad41848f88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2908a239-9a9c-424d-a25e-b52b320ef348" xmlns:ns4="14699dbd-23eb-47d5-a11a-8dab2a8bfb64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb120bc1534939806b9bc4170ddcf21" ns3:_="" ns4:_="">
     <xsd:import namespace="2908a239-9a9c-424d-a25e-b52b320ef348"/>
@@ -6881,6 +7090,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6891,23 +7106,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943795AF-9E85-4686-BF46-1A9E3F69B07A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{395500BF-5D64-47FA-8516-846D2479598F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6926,6 +7124,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943795AF-9E85-4686-BF46-1A9E3F69B07A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added and completed tests
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The king\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CA2729-2B78-4379-93F4-1A29A8143DEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Test Plan" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>TESTER COMMENTS</t>
   </si>
@@ -161,11 +162,26 @@
   <si>
     <t>When using both search bars simoultanously, it returns null with no entries right now(possible new task)</t>
   </si>
+  <si>
+    <t>Search with both search bars containing data simultaneuosly</t>
+  </si>
+  <si>
+    <t>user is disallowed and told about their error</t>
+  </si>
+  <si>
+    <t>User is told to only use one box to search</t>
+  </si>
+  <si>
+    <t>Put inappropriate format in both search boxes</t>
+  </si>
+  <si>
+    <t>User is disallowed and told about their error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -460,33 +476,9 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <strike/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <strike/>
@@ -893,7 +885,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,7 +929,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -957,7 +949,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3022,14 +3014,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="400050" cy="247650"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1144" name="Check Box 120" hidden="1">
@@ -3038,7 +3035,7 @@
                   <a14:compatExt spid="_x0000_s1144"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000078040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3078,7 +3075,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3406,16 +3403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:Y75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3956,7 +3953,7 @@
     </row>
     <row r="16" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14">
-        <v>43274</v>
+        <v>43865</v>
       </c>
       <c r="C16" s="25">
         <v>3</v>
@@ -3992,7 +3989,7 @@
     </row>
     <row r="17" spans="2:25" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
-        <v>43275</v>
+        <v>43865</v>
       </c>
       <c r="C17" s="25">
         <v>7</v>
@@ -4028,13 +4025,23 @@
     </row>
     <row r="18" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14">
-        <v>43276</v>
-      </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+        <v>43865</v>
+      </c>
+      <c r="C18" s="25">
+        <v>9</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="H18" s="16"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -4058,10 +4065,18 @@
       <c r="B19" s="14">
         <v>43277</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="C19" s="25">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15">
+        <v>4</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="G19" s="15"/>
       <c r="H19" s="16"/>
       <c r="I19" s="15"/>
@@ -5583,7 +5598,7 @@
     <mergeCell ref="B39:J39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B39:J39" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET"/>
+    <hyperlink ref="B39:J39" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -6866,11 +6881,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A2:B14"/>
+  <dimension ref="A2:B21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -6908,6 +6923,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6920,6 +6940,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E699AB3B5B90B4E9587B6CE8A7722F9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327bf17b6c8b56faa046bfad41848f88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2908a239-9a9c-424d-a25e-b52b320ef348" xmlns:ns4="14699dbd-23eb-47d5-a11a-8dab2a8bfb64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb120bc1534939806b9bc4170ddcf21" ns3:_="" ns4:_="">
     <xsd:import namespace="2908a239-9a9c-424d-a25e-b52b320ef348"/>
@@ -7090,36 +7125,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{395500BF-5D64-47FA-8516-846D2479598F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
-    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7142,9 +7151,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{395500BF-5D64-47FA-8516-846D2479598F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
+    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added new tests, some tests done
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2TestPlanV2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The king\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D9C36D-7694-439D-9AF3-B4151823AD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Test Plan" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>TESTER COMMENTS</t>
   </si>
@@ -193,13 +192,37 @@
     <t>Attempt to set the maximum price as -100</t>
   </si>
   <si>
-    <t>Error displayed to user</t>
+    <t>Set maximum price to 27000</t>
+  </si>
+  <si>
+    <t>Only Data entries with cost &lt;= 27000 are displayed</t>
+  </si>
+  <si>
+    <t>As expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential issue with labels leading to duplication, can maybe be resolved when map data is fully implemented. </t>
+  </si>
+  <si>
+    <t>Updating the price filter from 27000 to 29000</t>
+  </si>
+  <si>
+    <t>update display to show Data entries with cost &lt;= 29000</t>
+  </si>
+  <si>
+    <t>No results found</t>
+  </si>
+  <si>
+    <t>as expected</t>
+  </si>
+  <si>
+    <t>Maybe revisit code to prevent negative numbers as oppopsed to searchhing with them and returning no values.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -494,7 +517,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="5"/>
   </cellStyles>
   <dxfs count="35">
     <dxf>
@@ -947,11 +970,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -971,7 +994,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,11 +1014,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1011,11 +1034,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1031,7 +1054,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,7 +1078,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="'-Disclaimer-'!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3139,14 +3162,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
           <xdr:colOff>647700</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="400050" cy="247650"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1146" name="Check Box 122" hidden="1">
@@ -3195,7 +3223,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3523,7 +3551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
     <pageSetUpPr fitToPage="1"/>
@@ -3531,8 +3559,8 @@
   <dimension ref="B1:Y76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4107,7 +4135,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="2:25" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>43865</v>
       </c>
@@ -4121,12 +4149,18 @@
         <v>53</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="H17" s="16"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+      <c r="I17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -4267,14 +4301,28 @@
       <c r="B21" s="14">
         <v>43278</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="C21" s="25">
+        <v>3</v>
+      </c>
+      <c r="D21" s="15">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="H21" s="16"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="I21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>57</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -4295,13 +4343,25 @@
       <c r="B22" s="14">
         <v>43279</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="C22" s="25">
+        <v>3</v>
+      </c>
+      <c r="D22" s="15">
+        <v>5</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>56</v>
+      </c>
       <c r="H22" s="16"/>
-      <c r="I22" s="15"/>
+      <c r="I22" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="J22" s="15"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -5764,7 +5824,7 @@
     <mergeCell ref="B40:J40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B40:J40" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B40:J40" r:id="rId1" display="CLICK HERE TO CREATE IN SMARTSHEET"/>
   </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -7123,11 +7183,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A2:B22"/>
+  <dimension ref="A2:B24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -7165,6 +7225,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="b">
         <v>1</v>
@@ -7172,6 +7237,16 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7196,12 +7271,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001E699AB3B5B90B4E9587B6CE8A7722F9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327bf17b6c8b56faa046bfad41848f88">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2908a239-9a9c-424d-a25e-b52b320ef348" xmlns:ns4="14699dbd-23eb-47d5-a11a-8dab2a8bfb64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb120bc1534939806b9bc4170ddcf21" ns3:_="" ns4:_="">
     <xsd:import namespace="2908a239-9a9c-424d-a25e-b52b320ef348"/>
@@ -7372,6 +7441,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B01F70-A4AC-4F1F-BFEA-2CE3694CCB74}">
   <ds:schemaRefs>
@@ -7381,23 +7456,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943795AF-9E85-4686-BF46-1A9E3F69B07A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{395500BF-5D64-47FA-8516-846D2479598F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7414,4 +7472,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943795AF-9E85-4686-BF46-1A9E3F69B07A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2908a239-9a9c-424d-a25e-b52b320ef348"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="14699dbd-23eb-47d5-a11a-8dab2a8bfb64"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>